<commit_message>
Added initial descriptive statistics and cleaning
</commit_message>
<xml_diff>
--- a/data/NFHS Family Aggregation Variable List.xlsx
+++ b/data/NFHS Family Aggregation Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F32822-610A-4619-A384-7EDB8E73D434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4233E8-64F1-4D86-B07A-A2207A100B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5227" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5293" uniqueCount="1391">
   <si>
     <t>label</t>
   </si>
@@ -4089,13 +4089,127 @@
   </si>
   <si>
     <t>educationhh</t>
+  </si>
+  <si>
+    <t>s711</t>
+  </si>
+  <si>
+    <t>sm604</t>
+  </si>
+  <si>
+    <t>Mother Alive</t>
+  </si>
+  <si>
+    <t>Mother's line number</t>
+  </si>
+  <si>
+    <t>Father Alive</t>
+  </si>
+  <si>
+    <t>Father's line number</t>
+  </si>
+  <si>
+    <t>hv111</t>
+  </si>
+  <si>
+    <t>hv112</t>
+  </si>
+  <si>
+    <t>hv113</t>
+  </si>
+  <si>
+    <t>hv114</t>
+  </si>
+  <si>
+    <t>Relationship to household head</t>
+  </si>
+  <si>
+    <t>hv101</t>
+  </si>
+  <si>
+    <t>ever_married</t>
+  </si>
+  <si>
+    <t>male_sample</t>
+  </si>
+  <si>
+    <t>mother_alive</t>
+  </si>
+  <si>
+    <t>mother_linenumber</t>
+  </si>
+  <si>
+    <t>father_alive</t>
+  </si>
+  <si>
+    <t>father_linenumber</t>
+  </si>
+  <si>
+    <t>relationship_hh_head</t>
+  </si>
+  <si>
+    <t>total_adults_measured</t>
+  </si>
+  <si>
+    <t>Number of eligible men</t>
+  </si>
+  <si>
+    <t>Number of eligible women</t>
+  </si>
+  <si>
+    <t>Number of dejure members</t>
+  </si>
+  <si>
+    <t>Number of de facto members</t>
+  </si>
+  <si>
+    <t>Number of children under 5 years</t>
+  </si>
+  <si>
+    <t>hv010</t>
+  </si>
+  <si>
+    <t>hv011</t>
+  </si>
+  <si>
+    <t>hv012</t>
+  </si>
+  <si>
+    <t>hv013</t>
+  </si>
+  <si>
+    <t>hv014</t>
+  </si>
+  <si>
+    <t>neligible_men</t>
+  </si>
+  <si>
+    <t>neligible_women</t>
+  </si>
+  <si>
+    <t>ndejure_members</t>
+  </si>
+  <si>
+    <t>ndefacto_members</t>
+  </si>
+  <si>
+    <t>nchildren_under5</t>
+  </si>
+  <si>
+    <t>Head of household line number</t>
+  </si>
+  <si>
+    <t>hh_head_linenumber</t>
+  </si>
+  <si>
+    <t>hv218</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4120,6 +4234,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4555,13 +4675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BB052-C333-4DDF-AF33-13FC35516278}">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="E118" sqref="E118:G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5871,7 +5991,12 @@
       <c r="B76" t="s">
         <v>437</v>
       </c>
-      <c r="C76" s="2"/>
+      <c r="C76" s="2" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1354</v>
+      </c>
       <c r="E76" t="s">
         <v>377</v>
       </c>
@@ -6569,7 +6694,15 @@
       <c r="A115" t="s">
         <v>1245</v>
       </c>
-      <c r="B115" s="7"/>
+      <c r="B115" s="7" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E115" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F115" t="s">
+        <v>1246</v>
+      </c>
       <c r="G115" t="s">
         <v>1246</v>
       </c>
@@ -6578,7 +6711,15 @@
       <c r="A116" t="s">
         <v>1248</v>
       </c>
-      <c r="B116" s="7"/>
+      <c r="B116" s="7" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E116" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F116" t="s">
+        <v>1247</v>
+      </c>
       <c r="G116" t="s">
         <v>1247</v>
       </c>
@@ -6587,11 +6728,208 @@
       <c r="A117" t="s">
         <v>1244</v>
       </c>
+      <c r="B117" s="7" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F117" t="s">
+        <v>1249</v>
+      </c>
       <c r="G117" t="s">
         <v>1249</v>
       </c>
     </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F118" t="s">
+        <v>1390</v>
+      </c>
+      <c r="G118" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E119" t="s">
+        <v>1359</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1359</v>
+      </c>
+      <c r="G119" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E120" t="s">
+        <v>1360</v>
+      </c>
+      <c r="F120" t="s">
+        <v>1360</v>
+      </c>
+      <c r="G120" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1361</v>
+      </c>
+      <c r="F121" t="s">
+        <v>1361</v>
+      </c>
+      <c r="G121" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F122" t="s">
+        <v>1362</v>
+      </c>
+      <c r="G122" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F123" t="s">
+        <v>1364</v>
+      </c>
+      <c r="G123" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E124" t="s">
+        <v>1378</v>
+      </c>
+      <c r="F124" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G124" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F125" t="s">
+        <v>1379</v>
+      </c>
+      <c r="G125" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E126" t="s">
+        <v>1380</v>
+      </c>
+      <c r="F126" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G126" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E127" t="s">
+        <v>1381</v>
+      </c>
+      <c r="F127" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G127" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1382</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1382</v>
+      </c>
+      <c r="G128" t="s">
+        <v>1382</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B40:B47">
     <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Commits after initial draft of Methods
</commit_message>
<xml_diff>
--- a/data/NFHS Family Aggregation Variable List.xlsx
+++ b/data/NFHS Family Aggregation Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4233E8-64F1-4D86-B07A-A2207A100B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF48E729-6A19-45D0-AF5D-0BF8C3E17121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5293" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5295" uniqueCount="1393">
   <si>
     <t>label</t>
   </si>
@@ -4203,6 +4203,12 @@
   </si>
   <si>
     <t>hv218</t>
+  </si>
+  <si>
+    <t>marital3</t>
+  </si>
+  <si>
+    <t>Marital status 3</t>
   </si>
 </sst>
 </file>
@@ -4675,13 +4681,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BB052-C333-4DDF-AF33-13FC35516278}">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E118" sqref="E118:G118"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5237,12 +5243,6 @@
       <c r="D28" t="s">
         <v>195</v>
       </c>
-      <c r="E28" t="s">
-        <v>311</v>
-      </c>
-      <c r="F28" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
@@ -5260,1698 +5260,1712 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>1392</v>
       </c>
       <c r="B30" t="s">
-        <v>392</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" t="s">
-        <v>74</v>
+        <v>1391</v>
       </c>
       <c r="E30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F30" t="s">
-        <v>312</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>314</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>395</v>
+        <v>393</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B33" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>317</v>
       </c>
       <c r="B34" t="s">
-        <v>440</v>
-      </c>
-      <c r="C34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" t="s">
-        <v>82</v>
+        <v>394</v>
       </c>
       <c r="E34" t="s">
-        <v>445</v>
+        <v>316</v>
       </c>
       <c r="F34" t="s">
-        <v>445</v>
+        <v>316</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>441</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>442</v>
+        <v>440</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
       </c>
       <c r="E35" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F35" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>441</v>
       </c>
       <c r="B36" t="s">
-        <v>443</v>
-      </c>
-      <c r="C36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" t="s">
-        <v>83</v>
+        <v>442</v>
       </c>
       <c r="E36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>452</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>232</v>
+        <v>83</v>
       </c>
       <c r="E37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>452</v>
       </c>
       <c r="B38" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>231</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>232</v>
       </c>
       <c r="E38" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F38" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>453</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>234</v>
+        <v>84</v>
       </c>
       <c r="E39" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F39" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>453</v>
       </c>
       <c r="B40" t="s">
-        <v>1262</v>
+        <v>454</v>
       </c>
       <c r="C40" t="s">
-        <v>214</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E40" s="2"/>
+        <v>233</v>
+      </c>
+      <c r="D40" t="s">
+        <v>234</v>
+      </c>
+      <c r="E40" t="s">
+        <v>449</v>
+      </c>
+      <c r="F40" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>248</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C41" t="s">
-        <v>216</v>
-      </c>
-      <c r="D41" t="s">
-        <v>221</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>248</v>
       </c>
       <c r="B42" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C42" t="s">
-        <v>215</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="D42" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C43" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C44" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" t="s">
-        <v>225</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="B45" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C45" t="s">
-        <v>217</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E45" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="D45" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C46" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C48" t="s">
+        <v>220</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>134</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>396</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>154</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>144</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>372</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>135</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>1270</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>155</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>136</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>1271</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>156</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>137</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>1272</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>157</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>138</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>1273</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>158</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>139</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>1274</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>159</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>140</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>1275</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>160</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>141</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>1276</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>161</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>142</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>1277</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>162</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>143</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>1278</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>163</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>98</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>1279</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>97</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>1280</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>101</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>397</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>100</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
         <v>318</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>102</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>398</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>103</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E62" t="s">
         <v>319</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F62" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>180</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>399</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>320</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>4</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>400</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>56</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>321</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>278</v>
-      </c>
-      <c r="B64" t="s">
-        <v>401</v>
-      </c>
-      <c r="C64" t="s">
-        <v>279</v>
-      </c>
-      <c r="D64" t="s">
-        <v>293</v>
-      </c>
-      <c r="E64" t="s">
-        <v>322</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B65" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C65" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D65" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E65" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>324</v>
+        <v>280</v>
       </c>
       <c r="B66" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="C66" t="s">
+        <v>281</v>
+      </c>
+      <c r="D66" t="s">
+        <v>294</v>
       </c>
       <c r="E66" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B67" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E67" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>326</v>
       </c>
       <c r="B68" t="s">
-        <v>405</v>
-      </c>
-      <c r="C68" t="s">
-        <v>105</v>
+        <v>404</v>
       </c>
       <c r="E68" t="s">
-        <v>328</v>
-      </c>
-      <c r="F68" t="s">
-        <v>184</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B69" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E69" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C70" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E70" t="s">
-        <v>330</v>
+        <v>329</v>
+      </c>
+      <c r="F70" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B71" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E71" t="s">
-        <v>331</v>
-      </c>
-      <c r="F71" t="s">
-        <v>186</v>
+        <v>330</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E72" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>334</v>
+        <v>110</v>
       </c>
       <c r="B73" t="s">
-        <v>410</v>
+        <v>409</v>
+      </c>
+      <c r="C73" t="s">
+        <v>113</v>
       </c>
       <c r="E73" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F73" t="s">
-        <v>335</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>175</v>
+        <v>334</v>
+      </c>
+      <c r="B74" t="s">
+        <v>410</v>
+      </c>
+      <c r="E74" t="s">
+        <v>333</v>
+      </c>
+      <c r="F74" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>176</v>
-      </c>
-      <c r="B75" t="s">
-        <v>383</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D75" t="s">
-        <v>237</v>
-      </c>
-      <c r="E75" t="s">
-        <v>375</v>
-      </c>
-      <c r="F75" t="s">
-        <v>375</v>
+        <v>175</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>376</v>
+        <v>176</v>
       </c>
       <c r="B76" t="s">
-        <v>437</v>
+        <v>383</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>1353</v>
+        <v>235</v>
       </c>
       <c r="D76" t="s">
-        <v>1354</v>
+        <v>237</v>
       </c>
       <c r="E76" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F76" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>376</v>
       </c>
       <c r="B77" t="s">
-        <v>1291</v>
+        <v>437</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>236</v>
+        <v>1353</v>
       </c>
       <c r="D77" t="s">
-        <v>238</v>
+        <v>1354</v>
+      </c>
+      <c r="E77" t="s">
+        <v>377</v>
+      </c>
+      <c r="F77" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="B78" t="s">
-        <v>1282</v>
-      </c>
-      <c r="C78" t="s">
-        <v>124</v>
+        <v>1291</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="D78" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B79" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="C79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D79" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B80" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C80" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D80" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B81" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="C81" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B82" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C82" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D82" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B83" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="C83" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D84" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B85" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C85" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D85" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B86" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C86" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D86" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>419</v>
+        <v>1290</v>
       </c>
       <c r="C87" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D87" t="s">
-        <v>173</v>
-      </c>
-      <c r="E87" t="s">
-        <v>327</v>
-      </c>
-      <c r="F87" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>123</v>
+      </c>
+      <c r="B88" t="s">
+        <v>419</v>
+      </c>
+      <c r="C88" t="s">
+        <v>133</v>
+      </c>
+      <c r="D88" t="s">
+        <v>173</v>
+      </c>
+      <c r="E88" t="s">
+        <v>327</v>
+      </c>
+      <c r="F88" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>23</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="C89" t="s">
-        <v>63</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="G89" s="5"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>1292</v>
+        <v>411</v>
       </c>
       <c r="C90" t="s">
-        <v>247</v>
+        <v>63</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>249</v>
+        <v>81</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>223</v>
+        <v>24</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>412</v>
+        <v>1292</v>
       </c>
       <c r="C91" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>223</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C92" t="s">
+        <v>251</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="G92" s="5"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>290</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>291</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F93" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
+      <c r="G93" s="5"/>
+    </row>
+    <row r="94" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B94" s="7" t="s">
         <v>1293</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D94" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E94" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F94" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="G93" s="6"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>289</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="C94" t="s">
-        <v>268</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="G94" s="5"/>
+      <c r="G94" s="6"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>289</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C95" t="s">
-        <v>239</v>
-      </c>
-      <c r="D95" t="s">
-        <v>295</v>
-      </c>
-      <c r="E95" t="s">
-        <v>336</v>
-      </c>
-      <c r="F95" t="s">
-        <v>336</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C96" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D96" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E96" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F96" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D97" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E97" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F97" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C98" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D98" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E98" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F98" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C99" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D99" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="E99" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F99" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C100" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D100" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E100" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F100" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C101" t="s">
-        <v>62</v>
+        <v>244</v>
       </c>
       <c r="D101" t="s">
-        <v>80</v>
+        <v>283</v>
       </c>
       <c r="E101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>21</v>
+        <v>256</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C102" t="s">
-        <v>245</v>
+        <v>62</v>
       </c>
       <c r="D102" t="s">
-        <v>284</v>
+        <v>80</v>
       </c>
       <c r="E102" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F102" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C103" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D103" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E103" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F103" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>255</v>
+        <v>22</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C104" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D104" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="E104" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F104" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C105" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D105" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E105" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F105" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C106" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D106" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E106" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F106" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C107" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D107" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E107" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F107" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C108" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D108" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E108" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F108" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C109" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D109" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E109" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F109" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C110" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D110" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="E110" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F110" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C111" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D111" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E111" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F111" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>275</v>
+        <v>31</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C112" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D112" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="E112" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F112" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>275</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>413</v>
+        <v>434</v>
       </c>
       <c r="C113" t="s">
-        <v>276</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="G113" s="2"/>
+        <v>271</v>
+      </c>
+      <c r="D113" t="s">
+        <v>272</v>
+      </c>
+      <c r="E113" t="s">
+        <v>353</v>
+      </c>
+      <c r="F113" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>209</v>
+        <v>32</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="C114" t="s">
-        <v>210</v>
-      </c>
-      <c r="D114" t="s">
-        <v>211</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G114" s="2"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>1245</v>
+        <v>209</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>1365</v>
-      </c>
-      <c r="E115" t="s">
-        <v>1246</v>
-      </c>
-      <c r="F115" t="s">
-        <v>1246</v>
-      </c>
-      <c r="G115" t="s">
-        <v>1246</v>
+        <v>435</v>
+      </c>
+      <c r="C115" t="s">
+        <v>210</v>
+      </c>
+      <c r="D115" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E116" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="F116" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="G116" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>1244</v>
+        <v>1248</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="E117" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="F117" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="G117" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>1388</v>
+        <v>1244</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>1389</v>
+        <v>1372</v>
       </c>
       <c r="E118" t="s">
-        <v>1390</v>
+        <v>1249</v>
       </c>
       <c r="F118" t="s">
-        <v>1390</v>
+        <v>1249</v>
       </c>
       <c r="G118" t="s">
-        <v>1390</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>1355</v>
+        <v>1388</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>1367</v>
+        <v>1389</v>
       </c>
       <c r="E119" t="s">
-        <v>1359</v>
+        <v>1390</v>
       </c>
       <c r="F119" t="s">
-        <v>1359</v>
+        <v>1390</v>
       </c>
       <c r="G119" t="s">
-        <v>1359</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="E120" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="F120" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="G120" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="E121" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="F121" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="G121" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E122" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="F122" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="G122" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>1363</v>
+        <v>1358</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="E123" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="F123" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="G123" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>1373</v>
+        <v>1363</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>1383</v>
+        <v>1371</v>
       </c>
       <c r="E124" t="s">
-        <v>1378</v>
+        <v>1364</v>
       </c>
       <c r="F124" t="s">
-        <v>1378</v>
+        <v>1364</v>
       </c>
       <c r="G124" t="s">
-        <v>1378</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="E125" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="F125" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="G125" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="E126" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="F126" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G126" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="E127" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="F127" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="G127" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1381</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G128" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>1377</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B129" s="7" t="s">
         <v>1387</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E129" t="s">
         <v>1382</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F129" t="s">
         <v>1382</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G129" t="s">
         <v>1382</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B40:B47">
+  <conditionalFormatting sqref="B41:B48">
     <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48:B56">
+  <conditionalFormatting sqref="B49:B57">
     <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57:B58">
+  <conditionalFormatting sqref="B58:B59">
     <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
+  <conditionalFormatting sqref="B60">
     <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+  <conditionalFormatting sqref="B29:B30">
     <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B78:B87">
+  <conditionalFormatting sqref="B79:B88">
     <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
+  <conditionalFormatting sqref="B78">
     <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B89:B94">
+  <conditionalFormatting sqref="B90:B95">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>